<commit_message>
updated datasets for rev 2
</commit_message>
<xml_diff>
--- a/datasets/Beauchamp_2020_data.xlsx
+++ b/datasets/Beauchamp_2020_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10460" windowHeight="7410" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10463" windowHeight="7410" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ElectrodeOrder" sheetId="2" r:id="rId1"/>
@@ -669,14 +669,14 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="34.26953125" customWidth="1"/>
+    <col min="1" max="1" width="34.265625" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="4" max="4" width="36.7265625" customWidth="1"/>
+    <col min="4" max="4" width="36.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
@@ -699,7 +699,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -724,7 +724,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -749,7 +749,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -774,7 +774,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -799,7 +799,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -822,7 +822,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -845,7 +845,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -868,7 +868,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -891,7 +891,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -916,7 +916,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -941,7 +941,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -966,7 +966,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1001,18 +1001,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26:F34"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="27.08984375" customWidth="1"/>
-    <col min="2" max="2" width="30.26953125" customWidth="1"/>
-    <col min="10" max="10" width="19.54296875" customWidth="1"/>
+    <col min="1" max="1" width="27.06640625" customWidth="1"/>
+    <col min="2" max="2" width="30.265625" customWidth="1"/>
+    <col min="10" max="10" width="19.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>29</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1141,7 +1141,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1185,7 +1185,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1229,7 +1229,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1273,7 +1273,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1317,7 +1317,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1361,7 +1361,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1449,7 +1449,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1581,7 +1581,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1625,7 +1625,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -1713,7 +1713,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -1801,7 +1801,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -2065,7 +2065,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="26" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A26" s="5" t="s">
         <v>2</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="27" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A27" s="5" t="s">
         <v>2</v>
       </c>
@@ -2197,7 +2197,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="28" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A28" s="5" t="s">
         <v>2</v>
       </c>
@@ -2241,7 +2241,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="29" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A29" s="5" t="s">
         <v>2</v>
       </c>
@@ -2285,7 +2285,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="30" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A30" s="5" t="s">
         <v>2</v>
       </c>
@@ -2329,7 +2329,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="31" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A31" s="5" t="s">
         <v>2</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="32" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A32" s="5" t="s">
         <v>2</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="33" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A33" s="5" t="s">
         <v>2</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A34" s="5" t="s">
         <v>2</v>
       </c>
@@ -2505,7 +2505,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>2</v>
       </c>
@@ -2549,7 +2549,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>2</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>2</v>
       </c>
@@ -2637,7 +2637,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>2</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>2</v>
       </c>
@@ -2725,7 +2725,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>2</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>2</v>
       </c>
@@ -2813,7 +2813,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>2</v>
       </c>
@@ -2857,7 +2857,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>2</v>
       </c>
@@ -2901,7 +2901,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>2</v>
       </c>
@@ -2945,7 +2945,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>2</v>
       </c>
@@ -2989,7 +2989,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>2</v>
       </c>
@@ -3033,7 +3033,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>2</v>
       </c>
@@ -3077,7 +3077,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>2</v>
       </c>
@@ -3121,7 +3121,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>2</v>
       </c>
@@ -3165,7 +3165,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>2</v>
       </c>
@@ -3209,7 +3209,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>2</v>
       </c>
@@ -3253,7 +3253,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>2</v>
       </c>
@@ -3297,7 +3297,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>2</v>
       </c>
@@ -3341,7 +3341,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>2</v>
       </c>
@@ -3385,7 +3385,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>2</v>
       </c>
@@ -3429,7 +3429,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>2</v>
       </c>
@@ -3473,7 +3473,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>2</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>2</v>
       </c>

</xml_diff>